<commit_message>
IMPLEMENTAÇÃO KIT MANUTENÇÃO AJUSTES ETIQUETA KIT'S
</commit_message>
<xml_diff>
--- a/SIG/Producao/Producao/Modelos/REQUISICAO_KIT_MODELO.xlsx
+++ b/SIG/Producao/Producao/Modelos/REQUISICAO_KIT_MODELO.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\wognascimento\SIG\SIG\Producao\Producao\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9410B262-CC21-4128-B5E5-6D74548A8E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F748ED-79A0-451D-988B-6269D1516F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{795787B9-A603-4E9F-9555-87E07481D83A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="RELATÓRIO" sheetId="1" r:id="rId1"/>
+    <sheet name="ETIQUETA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$8:$O$8</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Planilha1!$8:$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RELATÓRIO!$A$8:$P$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">RELATÓRIO!$8:$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>QTD</t>
   </si>
@@ -97,6 +98,9 @@
   </si>
   <si>
     <t>NOITE MONTAGEM</t>
+  </si>
+  <si>
+    <t>OK Confere</t>
   </si>
 </sst>
 </file>
@@ -663,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC889DE-7B05-4795-BCD8-9882F919D78A}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:O8"/>
+      <selection activeCell="A8" sqref="A8:P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +682,7 @@
     <col min="15" max="15" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -696,7 +700,7 @@
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -714,7 +718,7 @@
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -736,7 +740,7 @@
       <c r="M3" s="17"/>
       <c r="N3" s="18"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
@@ -756,7 +760,7 @@
       <c r="M4" s="18"/>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -776,7 +780,7 @@
       <c r="M5" s="18"/>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="1:15" ht="32.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
@@ -794,7 +798,7 @@
       <c r="M6" s="25"/>
       <c r="N6" s="26"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
@@ -810,7 +814,7 @@
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -840,8 +844,11 @@
       <c r="O8" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -857,7 +864,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -873,7 +880,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -889,7 +896,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -905,7 +912,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -921,7 +928,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -937,7 +944,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -953,7 +960,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1226,8 +1233,8 @@
       <c r="N32" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="o5KNDkAULBei3lisWzFax5LsKdB8D6eXXy4lkN8FImC1AoAlMkOC6X8eLxOXZlwfz76uYnhwseag3VGR/43NQg==" saltValue="riuDnxJTWiYS75WvntNxGA==" spinCount="100000" sheet="1" autoFilter="0"/>
-  <autoFilter ref="A8:O8" xr:uid="{DCC889DE-7B05-4795-BCD8-9882F919D78A}">
+  <sheetProtection algorithmName="SHA-512" hashValue="70/idSwzFE+YHGcRNnMLMvL1/lMX81qWT/fmfk42ePtd1UTyrsNvDI957pIl99kIRbb7ZEllCMp6IWQBltDcBg==" saltValue="Bvqzu6kixWTMoRXDkEev5w==" spinCount="100000" sheet="1" autoFilter="0"/>
+  <autoFilter ref="A8:P8" xr:uid="{DCC889DE-7B05-4795-BCD8-9882F919D78A}">
     <filterColumn colId="2" showButton="0"/>
     <filterColumn colId="4" showButton="0"/>
     <filterColumn colId="5" showButton="0"/>
@@ -1265,9 +1272,23 @@
     <mergeCell ref="G4:I4"/>
   </mergeCells>
   <pageMargins left="3.937007874015748E-2" right="3.937007874015748E-2" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="99" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;R&amp;"-,Negrito"Impresso em:  &amp;D</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5928B491-0A4D-4494-BAC2-51FFA16B7264}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <sheetProtection algorithmName="SHA-512" hashValue="zAGxngdG27lZRaexr2cguOKjhpD6JhzfWo570S1uWFXpgfxziXW/FtNLXBUlULGHLAJiefx3cuYWTmbt2nk97Q==" saltValue="VBiHb9ndeVH/36aOhwDWjw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
IMPLEMENTAÇÃO APLICATIVO CONTROLADOS SHOPPING
</commit_message>
<xml_diff>
--- a/SIG/Producao/Producao/Modelos/REQUISICAO_KIT_MODELO.xlsx
+++ b/SIG/Producao/Producao/Modelos/REQUISICAO_KIT_MODELO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\wognascimento\SIG\SIG\Producao\Producao\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F748ED-79A0-451D-988B-6269D1516F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDC6182-1E5A-43AD-BB4E-EB8F08A2016B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{795787B9-A603-4E9F-9555-87E07481D83A}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="ETIQUETA" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RELATÓRIO!$A$8:$P$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RELATÓRIO!$A$8:$R$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">RELATÓRIO!$8:$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>QTD</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>OK Confere</t>
+  </si>
+  <si>
+    <t>V. UNIT.</t>
+  </si>
+  <si>
+    <t>PESO. UNIT.</t>
   </si>
 </sst>
 </file>
@@ -667,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC889DE-7B05-4795-BCD8-9882F919D78A}">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:P8"/>
+      <selection activeCell="A8" sqref="A8:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,9 +686,11 @@
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="8" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
@@ -700,7 +708,7 @@
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
@@ -718,7 +726,7 @@
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -740,7 +748,7 @@
       <c r="M3" s="17"/>
       <c r="N3" s="18"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
@@ -760,7 +768,7 @@
       <c r="M4" s="18"/>
       <c r="N4" s="5"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -780,7 +788,7 @@
       <c r="M5" s="18"/>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="1:16" ht="32.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
@@ -798,7 +806,7 @@
       <c r="M6" s="25"/>
       <c r="N6" s="26"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="27"/>
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
@@ -814,7 +822,7 @@
       <c r="M7" s="27"/>
       <c r="N7" s="27"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -847,8 +855,14 @@
       <c r="P8" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -864,7 +878,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -880,7 +894,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -896,7 +910,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -912,7 +926,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -928,7 +942,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -944,7 +958,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -960,7 +974,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1233,8 +1247,8 @@
       <c r="N32" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="70/idSwzFE+YHGcRNnMLMvL1/lMX81qWT/fmfk42ePtd1UTyrsNvDI957pIl99kIRbb7ZEllCMp6IWQBltDcBg==" saltValue="Bvqzu6kixWTMoRXDkEev5w==" spinCount="100000" sheet="1" autoFilter="0"/>
-  <autoFilter ref="A8:P8" xr:uid="{DCC889DE-7B05-4795-BCD8-9882F919D78A}">
+  <sheetProtection algorithmName="SHA-512" hashValue="zWCKb4A/m5MLcU7MdhwtmLGtdSGparEzAYB6yZ2Vy9gw3ZD93egewe+QCisIt1TTUXnn0AOzEPcYB+1Rm1BK5w==" saltValue="l3BILJnQRkRQsq72VcGdUQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" autoFilter="0"/>
+  <autoFilter ref="A8:R8" xr:uid="{DCC889DE-7B05-4795-BCD8-9882F919D78A}">
     <filterColumn colId="2" showButton="0"/>
     <filterColumn colId="4" showButton="0"/>
     <filterColumn colId="5" showButton="0"/>

</xml_diff>